<commit_message>
Restructure some of the overall algorithm, begin to fix errors in classifications of busses
</commit_message>
<xml_diff>
--- a/Program/data/system_basecase.xlsx
+++ b/Program/data/system_basecase.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Documents/Work/UW/Teaching/EE454/2021/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mtsti\Desktop\454_Project\UW_EE454_Power_Flow_Solver\Program\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1A68B2-B6F7-EB4A-AF68-ED7D8F86DC32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CFB01F4-E57E-4CDC-B77E-552576E2BFC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14746" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BusData" sheetId="1" r:id="rId1"/>
@@ -99,12 +99,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -147,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -158,6 +164,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,13 +447,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -466,7 +473,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -486,7 +493,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -506,7 +513,7 @@
         <v>1.0449999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -526,127 +533,127 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="4">
         <v>57.8</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="4">
         <v>-3.9</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="4">
         <v>7.6</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="4">
         <v>1.6</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="4">
         <v>13.5</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="4">
         <v>8.5</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
+      <c r="E7" s="4">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="4">
         <v>29.5</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="4">
         <v>13.6</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
+      <c r="E8" s="4">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="4">
         <v>9</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="4">
         <v>5.8</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="4">
         <v>4.3</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="4">
         <v>2.1</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
+      <c r="E10" s="4">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
@@ -666,27 +673,27 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="4">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="4">
         <v>13.5</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="4">
         <v>5.8</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
+      <c r="E12" s="4">
+        <v>0</v>
+      </c>
+      <c r="F12" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
@@ -716,18 +723,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="12.6640625" customWidth="1"/>
     <col min="4" max="5" width="13.6640625" customWidth="1"/>
     <col min="6" max="6" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -747,7 +754,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -767,7 +774,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>1</v>
       </c>
@@ -787,7 +794,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>2</v>
       </c>
@@ -807,7 +814,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>2</v>
       </c>
@@ -827,7 +834,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>2</v>
       </c>
@@ -847,7 +854,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>3</v>
       </c>
@@ -867,7 +874,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>4</v>
       </c>
@@ -887,7 +894,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9">
         <v>4</v>
       </c>
@@ -907,7 +914,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A10">
         <v>5</v>
       </c>
@@ -927,7 +934,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11">
         <v>6</v>
       </c>
@@ -947,7 +954,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12">
         <v>6</v>
       </c>
@@ -967,7 +974,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13">
         <v>6</v>
       </c>
@@ -987,7 +994,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14">
         <v>7</v>
       </c>
@@ -1007,7 +1014,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A15">
         <v>7</v>
       </c>
@@ -1027,7 +1034,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16">
         <v>8</v>
       </c>
@@ -1047,7 +1054,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A17">
         <v>10</v>
       </c>
@@ -1067,7 +1074,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A18">
         <v>11</v>
       </c>

</xml_diff>